<commit_message>
melhora de logica e mudanca de dados na base de dados
</commit_message>
<xml_diff>
--- a/trabalho de aed pokedex.xlsx
+++ b/trabalho de aed pokedex.xlsx
@@ -283,7 +283,7 @@
     <t xml:space="preserve">Alolan Sandslash</t>
   </si>
   <si>
-    <t xml:space="preserve">Nidoran♀</t>
+    <t xml:space="preserve">Nidoran Femea</t>
   </si>
   <si>
     <t xml:space="preserve">Poison Pin pokemon</t>
@@ -298,7 +298,7 @@
     <t xml:space="preserve">Drill pokemon</t>
   </si>
   <si>
-    <t xml:space="preserve">Nidoran♂</t>
+    <t xml:space="preserve">Nidoran Macho</t>
   </si>
   <si>
     <t xml:space="preserve">Nidorino</t>
@@ -5228,12 +5228,13 @@
   </sheetPr>
   <dimension ref="A1:P1029"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1015" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1033" activeCellId="0" sqref="M1033"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A167" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E45" activeCellId="0" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="21.74"/>
   </cols>
   <sheetData>

</xml_diff>